<commit_message>
add CPU vs Pallelize sheet
</commit_message>
<xml_diff>
--- a/Project.xlsx
+++ b/Project.xlsx
@@ -13,10 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
-    <sheet name="Parallelize vs Optimize" sheetId="8" r:id="rId2"/>
-    <sheet name="CPU" sheetId="3" r:id="rId3"/>
-    <sheet name="Parallelize" sheetId="4" r:id="rId4"/>
-    <sheet name="Optimize" sheetId="5" r:id="rId5"/>
+    <sheet name="CPU vs Parallelize" sheetId="9" r:id="rId2"/>
+    <sheet name="Parallelize vs Optimize" sheetId="8" r:id="rId3"/>
+    <sheet name="CPU" sheetId="3" r:id="rId4"/>
+    <sheet name="Parallelize" sheetId="4" r:id="rId5"/>
+    <sheet name="Optimize" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
   <si>
     <t>n</t>
   </si>
@@ -337,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -376,6 +377,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1047,6 +1057,568 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CPU vs Paralleize</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CPU vs Parallelize'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CPU vs Parallelize'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CPU vs Parallelize'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>433.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4038.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32906.800000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D86D-4807-9F1D-2364EECCB746}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CPU vs Parallelize'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallelize</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CPU vs Parallelize'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CPU vs Parallelize'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>45.759</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.3874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>598.9556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6070.8582000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D86D-4807-9F1D-2364EECCB746}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="494072608"/>
+        <c:axId val="494071296"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="494072608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of images</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="494071296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="494071296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="494072608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1682,6 +2254,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
@@ -2177,6 +2786,500 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2712,6 +3815,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{125AC382-3E57-463B-86AE-B5B976847A2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3054,7 +4200,7 @@
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,6 +4298,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12">
+        <f>CPU!H5</f>
+        <v>49</v>
+      </c>
+      <c r="D4" s="19">
+        <f>Parallelize!H7</f>
+        <v>45.759</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12">
+        <f>CPU!H9</f>
+        <v>433.6</v>
+      </c>
+      <c r="D5" s="19">
+        <f>Parallelize!H13</f>
+        <v>95.3874</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>100</v>
+      </c>
+      <c r="C6" s="12">
+        <f>CPU!H13</f>
+        <v>4038.4</v>
+      </c>
+      <c r="D6" s="19">
+        <f>Parallelize!H19</f>
+        <v>598.9556</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="20">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="14">
+        <f>CPU!H17</f>
+        <v>32906.800000000003</v>
+      </c>
+      <c r="D7" s="21">
+        <f>Parallelize!H25</f>
+        <v>6070.8582000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D7"/>
   <sheetViews>
@@ -3234,7 +4463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H17"/>
   <sheetViews>
@@ -3249,15 +4478,15 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -3309,15 +4538,15 @@
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24">
+      <c r="B7" s="27">
         <v>10</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -3369,15 +4598,15 @@
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24">
+      <c r="B11" s="27">
         <v>100</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -3429,15 +4658,15 @@
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24">
+      <c r="B15" s="27">
         <v>1000</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
@@ -3498,7 +4727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H25"/>
   <sheetViews>
@@ -3513,15 +4742,15 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -3621,15 +4850,15 @@
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24">
+      <c r="B9" s="27">
         <v>10</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -3729,15 +4958,15 @@
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24">
+      <c r="B15" s="27">
         <v>100</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
@@ -3837,15 +5066,15 @@
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="27">
+      <c r="B21" s="30">
         <v>1000</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
@@ -3954,7 +5183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H29"/>
   <sheetViews>
@@ -3969,15 +5198,15 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -4101,15 +5330,15 @@
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24">
+      <c r="B10" s="27">
         <v>10</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -4233,15 +5462,15 @@
     </row>
     <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="24">
+      <c r="B17" s="27">
         <v>100</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
@@ -4365,15 +5594,15 @@
     </row>
     <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="27">
+      <c r="B24" s="30">
         <v>1000</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="32"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">

</xml_diff>

<commit_message>
add data comparison sheets
</commit_message>
<xml_diff>
--- a/Project.xlsx
+++ b/Project.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveS\OneDrive - Seneca College of Applied Arts &amp; Technology\GPU610\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git\CUDA_raytrace\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18510" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18510" windowHeight="12420" tabRatio="770" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="CPU" sheetId="3" r:id="rId4"/>
     <sheet name="Parallelize" sheetId="4" r:id="rId5"/>
     <sheet name="Optimize" sheetId="5" r:id="rId6"/>
+    <sheet name="Data C vs P" sheetId="11" r:id="rId7"/>
+    <sheet name="Data P vs O" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="12">
   <si>
     <t>n</t>
   </si>
@@ -37,25 +39,34 @@
     <t>CPU</t>
   </si>
   <si>
-    <t>Render</t>
-  </si>
-  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Malloc</t>
-  </si>
-  <si>
-    <t>Memcpy</t>
-  </si>
-  <si>
-    <t>MemcpyToSymbol</t>
   </si>
   <si>
     <t>Parallelize</t>
   </si>
   <si>
     <t>Optimize</t>
+  </si>
+  <si>
+    <t>render()</t>
+  </si>
+  <si>
+    <t>cudaMalloc()</t>
+  </si>
+  <si>
+    <t>cudaMemcpy()</t>
+  </si>
+  <si>
+    <t>cudaMemcpyToSymbol()</t>
+  </si>
+  <si>
+    <t>CPU (Milliseconds)</t>
+  </si>
+  <si>
+    <t>Parallelize (Milliseconds)</t>
+  </si>
+  <si>
+    <t>Optimize (Milliseconds)</t>
   </si>
 </sst>
 </file>
@@ -65,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +84,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,8 +119,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -334,11 +366,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -402,6 +508,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4199,7 +4344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -4217,10 +4362,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -4319,7 +4464,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -4399,10 +4544,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -4468,7 +4613,7 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4490,7 +4635,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
         <v>44</v>
@@ -4514,7 +4659,7 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>49</v>
@@ -4550,7 +4695,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>407</v>
@@ -4574,7 +4719,7 @@
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
         <v>430</v>
@@ -4610,7 +4755,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4">
         <v>3856</v>
@@ -4634,7 +4779,7 @@
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
         <v>4037</v>
@@ -4670,7 +4815,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16" s="4">
         <v>31194</v>
@@ -4694,7 +4839,7 @@
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>33030</v>
@@ -4732,12 +4877,12 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="B3" sqref="B3:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4754,7 +4899,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="10">
         <v>34.780999999999999</v>
@@ -4778,7 +4923,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="12">
         <v>2.0710000000000002</v>
@@ -4802,7 +4947,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" s="12">
         <v>1.0349999999999999</v>
@@ -4826,7 +4971,7 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="14">
         <v>45.283999999999999</v>
@@ -4862,7 +5007,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" s="10">
         <v>38.149000000000001</v>
@@ -4886,7 +5031,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="12">
         <v>17.181000000000001</v>
@@ -4910,7 +5055,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" s="12">
         <v>10.071</v>
@@ -4934,7 +5079,7 @@
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="14">
         <v>96.549000000000007</v>
@@ -4970,7 +5115,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" s="10">
         <v>35.848999999999997</v>
@@ -4994,7 +5139,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="12">
         <v>156.28</v>
@@ -5018,7 +5163,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="12">
         <v>91.578999999999994</v>
@@ -5042,7 +5187,7 @@
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="14">
         <v>549.27800000000002</v>
@@ -5077,8 +5222,8 @@
       <c r="H21" s="32"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>4</v>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C22" s="22">
         <v>34.709000000000003</v>
@@ -5102,7 +5247,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C23" s="22">
         <v>1447.758</v>
@@ -5126,7 +5271,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24" s="22">
         <v>789.12300000000005</v>
@@ -5150,7 +5295,7 @@
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="23">
         <v>5915.4319999999998</v>
@@ -5188,12 +5333,12 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="B3" sqref="B3:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5210,7 +5355,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="10">
         <v>0.35299999999999998</v>
@@ -5234,7 +5379,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="12">
         <v>34.529000000000003</v>
@@ -5258,7 +5403,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6" s="12">
         <v>1.7689999999999999</v>
@@ -5282,7 +5427,7 @@
     </row>
     <row r="7" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="12">
         <v>0.77500000000000002</v>
@@ -5306,7 +5451,7 @@
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="14">
         <v>44.829000000000001</v>
@@ -5342,7 +5487,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" s="10">
         <v>0.34499999999999997</v>
@@ -5366,7 +5511,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12" s="12">
         <v>35.271000000000001</v>
@@ -5390,7 +5535,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="12">
         <v>14.253</v>
@@ -5414,7 +5559,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C14" s="12">
         <v>7.4119999999999999</v>
@@ -5438,7 +5583,7 @@
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="14">
         <v>91.284999999999997</v>
@@ -5474,7 +5619,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" s="10">
         <v>0.36</v>
@@ -5498,7 +5643,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19" s="12">
         <v>34.170999999999999</v>
@@ -5522,7 +5667,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="12">
         <v>132.643</v>
@@ -5546,7 +5691,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" s="12">
         <v>67.117000000000004</v>
@@ -5570,7 +5715,7 @@
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="14">
         <v>526.38599999999997</v>
@@ -5605,8 +5750,8 @@
       <c r="H24" s="32"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>4</v>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C25" s="22">
         <v>0.36199999999999999</v>
@@ -5630,7 +5775,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C26" s="22">
         <v>34.347999999999999</v>
@@ -5654,7 +5799,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C27" s="22">
         <v>1215.6990000000001</v>
@@ -5678,7 +5823,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C28" s="22">
         <v>559.71600000000001</v>
@@ -5702,7 +5847,7 @@
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="23">
         <v>5100.2120000000004</v>
@@ -5733,4 +5878,1645 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="44"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="33">
+        <v>1</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
+      <c r="J4" s="33">
+        <v>1</v>
+      </c>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="35"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4">
+        <v>44</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43</v>
+      </c>
+      <c r="F5" s="4">
+        <v>44</v>
+      </c>
+      <c r="G5" s="4">
+        <v>43</v>
+      </c>
+      <c r="H5" s="7">
+        <f>AVERAGE(C5:G5)</f>
+        <v>43.6</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="10">
+        <v>34.780999999999999</v>
+      </c>
+      <c r="L5" s="10">
+        <v>37.122</v>
+      </c>
+      <c r="M5" s="10">
+        <v>34.631999999999998</v>
+      </c>
+      <c r="N5" s="10">
+        <v>34.505000000000003</v>
+      </c>
+      <c r="O5" s="10">
+        <v>35.536000000000001</v>
+      </c>
+      <c r="P5" s="11">
+        <f>AVERAGE(K5:O5)</f>
+        <v>35.315199999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3">
+        <v>49</v>
+      </c>
+      <c r="G6" s="3">
+        <v>49</v>
+      </c>
+      <c r="H6" s="42">
+        <f>AVERAGE(C6:G6)</f>
+        <v>49</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="12">
+        <v>2.0710000000000002</v>
+      </c>
+      <c r="L6" s="12">
+        <v>2.0670000000000002</v>
+      </c>
+      <c r="M6" s="12">
+        <v>2.052</v>
+      </c>
+      <c r="N6" s="12">
+        <v>2.052</v>
+      </c>
+      <c r="O6" s="12">
+        <v>2.125</v>
+      </c>
+      <c r="P6" s="13">
+        <f t="shared" ref="P6:P8" si="0">AVERAGE(K6:O6)</f>
+        <v>2.0733999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="L7" s="12">
+        <v>1.056</v>
+      </c>
+      <c r="M7" s="12">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="N7" s="12">
+        <v>1.0580000000000001</v>
+      </c>
+      <c r="O7" s="12">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="P7" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0486</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="14">
+        <v>45.283999999999999</v>
+      </c>
+      <c r="L8" s="14">
+        <v>47.780999999999999</v>
+      </c>
+      <c r="M8" s="14">
+        <v>44.82</v>
+      </c>
+      <c r="N8" s="14">
+        <v>44.73</v>
+      </c>
+      <c r="O8" s="14">
+        <v>46.18</v>
+      </c>
+      <c r="P8" s="43">
+        <f t="shared" si="0"/>
+        <v>45.759</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="36">
+        <v>10</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="J10" s="33">
+        <v>10</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="35"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>407</v>
+      </c>
+      <c r="D11" s="4">
+        <v>410</v>
+      </c>
+      <c r="E11" s="4">
+        <v>410</v>
+      </c>
+      <c r="F11" s="4">
+        <v>407</v>
+      </c>
+      <c r="G11" s="4">
+        <v>407</v>
+      </c>
+      <c r="H11" s="7">
+        <f>AVERAGE(C11:G11)</f>
+        <v>408.2</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="10">
+        <v>38.149000000000001</v>
+      </c>
+      <c r="L11" s="10">
+        <v>34.712000000000003</v>
+      </c>
+      <c r="M11" s="10">
+        <v>37.226999999999997</v>
+      </c>
+      <c r="N11" s="10">
+        <v>34.987000000000002</v>
+      </c>
+      <c r="O11" s="10">
+        <v>39.718000000000004</v>
+      </c>
+      <c r="P11" s="11">
+        <f>AVERAGE(K11:O11)</f>
+        <v>36.958600000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>430</v>
+      </c>
+      <c r="D12" s="3">
+        <v>434</v>
+      </c>
+      <c r="E12" s="3">
+        <v>437</v>
+      </c>
+      <c r="F12" s="3">
+        <v>434</v>
+      </c>
+      <c r="G12" s="3">
+        <v>433</v>
+      </c>
+      <c r="H12" s="42">
+        <f>AVERAGE(C12:G12)</f>
+        <v>433.6</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="12">
+        <v>17.181000000000001</v>
+      </c>
+      <c r="L12" s="12">
+        <v>17.170000000000002</v>
+      </c>
+      <c r="M12" s="12">
+        <v>16.951000000000001</v>
+      </c>
+      <c r="N12" s="12">
+        <v>17.006</v>
+      </c>
+      <c r="O12" s="12">
+        <v>17.096</v>
+      </c>
+      <c r="P12" s="13">
+        <f t="shared" ref="P12:P14" si="1">AVERAGE(K12:O12)</f>
+        <v>17.0808</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="12">
+        <v>10.071</v>
+      </c>
+      <c r="L13" s="12">
+        <v>10.084</v>
+      </c>
+      <c r="M13" s="12">
+        <v>10.1</v>
+      </c>
+      <c r="N13" s="12">
+        <v>10.087999999999999</v>
+      </c>
+      <c r="O13" s="12">
+        <v>10.118</v>
+      </c>
+      <c r="P13" s="13">
+        <f t="shared" si="1"/>
+        <v>10.092200000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="14">
+        <v>96.549000000000007</v>
+      </c>
+      <c r="L14" s="14">
+        <v>93.692999999999998</v>
+      </c>
+      <c r="M14" s="14">
+        <v>95.841999999999999</v>
+      </c>
+      <c r="N14" s="14">
+        <v>93.887</v>
+      </c>
+      <c r="O14" s="14">
+        <v>96.965999999999994</v>
+      </c>
+      <c r="P14" s="43">
+        <f t="shared" si="1"/>
+        <v>95.3874</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36">
+        <v>100</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
+      <c r="J16" s="33">
+        <v>100</v>
+      </c>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="35"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>3856</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3854</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3844</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3843</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3862</v>
+      </c>
+      <c r="H17" s="7">
+        <f>AVERAGE(C17:G17)</f>
+        <v>3851.8</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="10">
+        <v>35.848999999999997</v>
+      </c>
+      <c r="L17" s="10">
+        <v>37.28</v>
+      </c>
+      <c r="M17" s="10">
+        <v>34.792999999999999</v>
+      </c>
+      <c r="N17" s="10">
+        <v>34.597999999999999</v>
+      </c>
+      <c r="O17" s="10">
+        <v>37.707999999999998</v>
+      </c>
+      <c r="P17" s="11">
+        <f>AVERAGE(K17:O17)</f>
+        <v>36.045599999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4037</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4039</v>
+      </c>
+      <c r="E18" s="3">
+        <v>4030</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4037</v>
+      </c>
+      <c r="G18" s="3">
+        <v>4049</v>
+      </c>
+      <c r="H18" s="42">
+        <f>AVERAGE(C18:G18)</f>
+        <v>4038.4</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="12">
+        <v>156.28</v>
+      </c>
+      <c r="L18" s="12">
+        <v>160.30199999999999</v>
+      </c>
+      <c r="M18" s="12">
+        <v>158.09</v>
+      </c>
+      <c r="N18" s="12">
+        <v>157.66800000000001</v>
+      </c>
+      <c r="O18" s="12">
+        <v>158.69900000000001</v>
+      </c>
+      <c r="P18" s="13">
+        <f t="shared" ref="P18:P20" si="2">AVERAGE(K18:O18)</f>
+        <v>158.20779999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="12">
+        <v>91.578999999999994</v>
+      </c>
+      <c r="L19" s="12">
+        <v>92.361999999999995</v>
+      </c>
+      <c r="M19" s="12">
+        <v>92.37</v>
+      </c>
+      <c r="N19" s="12">
+        <v>92.984999999999999</v>
+      </c>
+      <c r="O19" s="12">
+        <v>93.004000000000005</v>
+      </c>
+      <c r="P19" s="13">
+        <f t="shared" si="2"/>
+        <v>92.460000000000008</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="14">
+        <v>549.27800000000002</v>
+      </c>
+      <c r="L20" s="14">
+        <v>555.48</v>
+      </c>
+      <c r="M20" s="14">
+        <v>678.98900000000003</v>
+      </c>
+      <c r="N20" s="14">
+        <v>651.87099999999998</v>
+      </c>
+      <c r="O20" s="14">
+        <v>559.16</v>
+      </c>
+      <c r="P20" s="43">
+        <f t="shared" si="2"/>
+        <v>598.9556</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="36">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="J22" s="39">
+        <v>1000</v>
+      </c>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>31194</v>
+      </c>
+      <c r="D23" s="4">
+        <v>31119</v>
+      </c>
+      <c r="E23" s="4">
+        <v>31108</v>
+      </c>
+      <c r="F23" s="4">
+        <v>31082</v>
+      </c>
+      <c r="G23" s="4">
+        <v>31151</v>
+      </c>
+      <c r="H23" s="7">
+        <f>AVERAGE(C23:G23)</f>
+        <v>31130.799999999999</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="22">
+        <v>34.709000000000003</v>
+      </c>
+      <c r="L23" s="12">
+        <v>38.118000000000002</v>
+      </c>
+      <c r="M23" s="22">
+        <v>34.709000000000003</v>
+      </c>
+      <c r="N23" s="12">
+        <v>36.225000000000001</v>
+      </c>
+      <c r="O23" s="12">
+        <v>38.567999999999998</v>
+      </c>
+      <c r="P23" s="13">
+        <f>AVERAGE(K23:O23)</f>
+        <v>36.465800000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>33030</v>
+      </c>
+      <c r="D24" s="3">
+        <v>32842</v>
+      </c>
+      <c r="E24" s="3">
+        <v>32838</v>
+      </c>
+      <c r="F24" s="3">
+        <v>32894</v>
+      </c>
+      <c r="G24" s="3">
+        <v>32930</v>
+      </c>
+      <c r="H24" s="42">
+        <f>AVERAGE(C24:G24)</f>
+        <v>32906.800000000003</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="22">
+        <v>1447.758</v>
+      </c>
+      <c r="L24" s="12">
+        <v>1453.61</v>
+      </c>
+      <c r="M24" s="22">
+        <v>1447.758</v>
+      </c>
+      <c r="N24" s="12">
+        <v>1435.3219999999999</v>
+      </c>
+      <c r="O24" s="12">
+        <v>1438.5519999999999</v>
+      </c>
+      <c r="P24" s="13">
+        <f t="shared" ref="P24:P26" si="3">AVERAGE(K24:O24)</f>
+        <v>1444.6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25" s="22">
+        <v>789.12300000000005</v>
+      </c>
+      <c r="L25" s="12">
+        <v>790.81</v>
+      </c>
+      <c r="M25" s="22">
+        <v>789.12300000000005</v>
+      </c>
+      <c r="N25" s="12">
+        <v>780.77499999999998</v>
+      </c>
+      <c r="O25" s="12">
+        <v>778.67399999999998</v>
+      </c>
+      <c r="P25" s="13">
+        <f t="shared" si="3"/>
+        <v>785.70100000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="23">
+        <v>5915.4319999999998</v>
+      </c>
+      <c r="L26" s="14">
+        <v>6030.924</v>
+      </c>
+      <c r="M26" s="23">
+        <v>5915.4319999999998</v>
+      </c>
+      <c r="N26" s="14">
+        <v>6659.2470000000003</v>
+      </c>
+      <c r="O26" s="14">
+        <v>5833.2560000000003</v>
+      </c>
+      <c r="P26" s="43">
+        <f t="shared" si="3"/>
+        <v>6070.8582000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J22:P22"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="J16:P16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="44"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36">
+        <v>1</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="J4" s="36">
+        <v>1</v>
+      </c>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="38"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="10">
+        <v>34.780999999999999</v>
+      </c>
+      <c r="D5" s="10">
+        <v>37.122</v>
+      </c>
+      <c r="E5" s="10">
+        <v>34.631999999999998</v>
+      </c>
+      <c r="F5" s="10">
+        <v>34.505000000000003</v>
+      </c>
+      <c r="G5" s="10">
+        <v>35.536000000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <f>AVERAGE(C5:G5)</f>
+        <v>35.315199999999997</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="O5" s="10">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="P5" s="11">
+        <f>AVERAGE(K5:O5)</f>
+        <v>0.3498</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12">
+        <v>2.0710000000000002</v>
+      </c>
+      <c r="D6" s="12">
+        <v>2.0670000000000002</v>
+      </c>
+      <c r="E6" s="12">
+        <v>2.052</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2.052</v>
+      </c>
+      <c r="G6" s="12">
+        <v>2.125</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ref="H6:H8" si="0">AVERAGE(C6:G6)</f>
+        <v>2.0733999999999999</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="12">
+        <v>34.529000000000003</v>
+      </c>
+      <c r="L6" s="12">
+        <v>36.249000000000002</v>
+      </c>
+      <c r="M6" s="12">
+        <v>36.715000000000003</v>
+      </c>
+      <c r="N6" s="12">
+        <v>34.183</v>
+      </c>
+      <c r="O6" s="12">
+        <v>37.442</v>
+      </c>
+      <c r="P6" s="13">
+        <f t="shared" ref="P6:P9" si="1">AVERAGE(K6:O6)</f>
+        <v>35.823600000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1.056</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1.0580000000000001</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0486</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="L7" s="12">
+        <v>1.76</v>
+      </c>
+      <c r="M7" s="12">
+        <v>1.9279999999999999</v>
+      </c>
+      <c r="N7" s="12">
+        <v>1.825</v>
+      </c>
+      <c r="O7" s="12">
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="P7" s="13">
+        <f t="shared" si="1"/>
+        <v>1.8134000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>45.283999999999999</v>
+      </c>
+      <c r="D8" s="14">
+        <v>47.780999999999999</v>
+      </c>
+      <c r="E8" s="14">
+        <v>44.82</v>
+      </c>
+      <c r="F8" s="14">
+        <v>44.73</v>
+      </c>
+      <c r="G8" s="14">
+        <v>46.18</v>
+      </c>
+      <c r="H8" s="43">
+        <f t="shared" si="0"/>
+        <v>45.759</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="M8" s="12">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="O8" s="12">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="P8" s="13">
+        <f t="shared" si="1"/>
+        <v>0.78079999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="14">
+        <v>44.829000000000001</v>
+      </c>
+      <c r="L9" s="14">
+        <v>46.637999999999998</v>
+      </c>
+      <c r="M9" s="14">
+        <v>47.222000000000001</v>
+      </c>
+      <c r="N9" s="14">
+        <v>44.610999999999997</v>
+      </c>
+      <c r="O9" s="14">
+        <v>47.656999999999996</v>
+      </c>
+      <c r="P9" s="43">
+        <f t="shared" si="1"/>
+        <v>46.191400000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="36">
+        <v>10</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="J11" s="33">
+        <v>10</v>
+      </c>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="35"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="10">
+        <v>38.149000000000001</v>
+      </c>
+      <c r="D12" s="10">
+        <v>34.712000000000003</v>
+      </c>
+      <c r="E12" s="10">
+        <v>37.226999999999997</v>
+      </c>
+      <c r="F12" s="10">
+        <v>34.987000000000002</v>
+      </c>
+      <c r="G12" s="10">
+        <v>39.718000000000004</v>
+      </c>
+      <c r="H12" s="11">
+        <f>AVERAGE(C12:G12)</f>
+        <v>36.958600000000004</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="O12" s="10">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="P12" s="11">
+        <f>AVERAGE(K12:O12)</f>
+        <v>0.34059999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12">
+        <v>17.181000000000001</v>
+      </c>
+      <c r="D13" s="12">
+        <v>17.170000000000002</v>
+      </c>
+      <c r="E13" s="12">
+        <v>16.951000000000001</v>
+      </c>
+      <c r="F13" s="12">
+        <v>17.006</v>
+      </c>
+      <c r="G13" s="12">
+        <v>17.096</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" ref="H13:H15" si="2">AVERAGE(C13:G13)</f>
+        <v>17.0808</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="12">
+        <v>35.271000000000001</v>
+      </c>
+      <c r="L13" s="12">
+        <v>34.139000000000003</v>
+      </c>
+      <c r="M13" s="12">
+        <v>36.978999999999999</v>
+      </c>
+      <c r="N13" s="12">
+        <v>36.332999999999998</v>
+      </c>
+      <c r="O13" s="12">
+        <v>37.576999999999998</v>
+      </c>
+      <c r="P13" s="13">
+        <f t="shared" ref="P13:P16" si="3">AVERAGE(K13:O13)</f>
+        <v>36.059799999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="12">
+        <v>10.071</v>
+      </c>
+      <c r="D14" s="12">
+        <v>10.084</v>
+      </c>
+      <c r="E14" s="12">
+        <v>10.1</v>
+      </c>
+      <c r="F14" s="12">
+        <v>10.087999999999999</v>
+      </c>
+      <c r="G14" s="12">
+        <v>10.118</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" si="2"/>
+        <v>10.092200000000002</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="12">
+        <v>14.253</v>
+      </c>
+      <c r="L14" s="12">
+        <v>14.518000000000001</v>
+      </c>
+      <c r="M14" s="12">
+        <v>14.765000000000001</v>
+      </c>
+      <c r="N14" s="12">
+        <v>14.879</v>
+      </c>
+      <c r="O14" s="12">
+        <v>14.393000000000001</v>
+      </c>
+      <c r="P14" s="13">
+        <f t="shared" si="3"/>
+        <v>14.561599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14">
+        <v>96.549000000000007</v>
+      </c>
+      <c r="D15" s="14">
+        <v>93.692999999999998</v>
+      </c>
+      <c r="E15" s="14">
+        <v>95.841999999999999</v>
+      </c>
+      <c r="F15" s="14">
+        <v>93.887</v>
+      </c>
+      <c r="G15" s="14">
+        <v>96.965999999999994</v>
+      </c>
+      <c r="H15" s="43">
+        <f t="shared" si="2"/>
+        <v>95.3874</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="12">
+        <v>7.4119999999999999</v>
+      </c>
+      <c r="L15" s="12">
+        <v>7.4370000000000003</v>
+      </c>
+      <c r="M15" s="12">
+        <v>7.4640000000000004</v>
+      </c>
+      <c r="N15" s="12">
+        <v>7.516</v>
+      </c>
+      <c r="O15" s="12">
+        <v>7.49</v>
+      </c>
+      <c r="P15" s="13">
+        <f t="shared" si="3"/>
+        <v>7.4638000000000009</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="14">
+        <v>91.284999999999997</v>
+      </c>
+      <c r="L16" s="14">
+        <v>90.652000000000001</v>
+      </c>
+      <c r="M16" s="14">
+        <v>93.912000000000006</v>
+      </c>
+      <c r="N16" s="14">
+        <v>92.986000000000004</v>
+      </c>
+      <c r="O16" s="14">
+        <v>92.966999999999999</v>
+      </c>
+      <c r="P16" s="43">
+        <f t="shared" si="3"/>
+        <v>92.360399999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36">
+        <v>100</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="J18" s="33">
+        <v>100</v>
+      </c>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="35"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="10">
+        <v>35.848999999999997</v>
+      </c>
+      <c r="D19" s="10">
+        <v>37.28</v>
+      </c>
+      <c r="E19" s="10">
+        <v>34.792999999999999</v>
+      </c>
+      <c r="F19" s="10">
+        <v>34.597999999999999</v>
+      </c>
+      <c r="G19" s="10">
+        <v>37.707999999999998</v>
+      </c>
+      <c r="H19" s="11">
+        <f>AVERAGE(C19:G19)</f>
+        <v>36.045599999999993</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="L19" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="M19" s="10">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="N19" s="10">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="P19" s="11">
+        <f>AVERAGE(K19:O19)</f>
+        <v>0.34459999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12">
+        <v>156.28</v>
+      </c>
+      <c r="D20" s="12">
+        <v>160.30199999999999</v>
+      </c>
+      <c r="E20" s="12">
+        <v>158.09</v>
+      </c>
+      <c r="F20" s="12">
+        <v>157.66800000000001</v>
+      </c>
+      <c r="G20" s="12">
+        <v>158.69900000000001</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" ref="H20:H22" si="4">AVERAGE(C20:G20)</f>
+        <v>158.20779999999999</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="12">
+        <v>34.170999999999999</v>
+      </c>
+      <c r="L20" s="12">
+        <v>34.698</v>
+      </c>
+      <c r="M20" s="12">
+        <v>36.082000000000001</v>
+      </c>
+      <c r="N20" s="12">
+        <v>34.481000000000002</v>
+      </c>
+      <c r="O20" s="12">
+        <v>35.457000000000001</v>
+      </c>
+      <c r="P20" s="13">
+        <f t="shared" ref="P20:P23" si="5">AVERAGE(K20:O20)</f>
+        <v>34.977799999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="12">
+        <v>91.578999999999994</v>
+      </c>
+      <c r="D21" s="12">
+        <v>92.361999999999995</v>
+      </c>
+      <c r="E21" s="12">
+        <v>92.37</v>
+      </c>
+      <c r="F21" s="12">
+        <v>92.984999999999999</v>
+      </c>
+      <c r="G21" s="12">
+        <v>93.004000000000005</v>
+      </c>
+      <c r="H21" s="13">
+        <f t="shared" si="4"/>
+        <v>92.460000000000008</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="12">
+        <v>132.643</v>
+      </c>
+      <c r="L21" s="12">
+        <v>133.92400000000001</v>
+      </c>
+      <c r="M21" s="12">
+        <v>135.04900000000001</v>
+      </c>
+      <c r="N21" s="12">
+        <v>133.21299999999999</v>
+      </c>
+      <c r="O21" s="12">
+        <v>131.80500000000001</v>
+      </c>
+      <c r="P21" s="13">
+        <f t="shared" si="5"/>
+        <v>133.32679999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14">
+        <v>549.27800000000002</v>
+      </c>
+      <c r="D22" s="14">
+        <v>555.48</v>
+      </c>
+      <c r="E22" s="14">
+        <v>678.98900000000003</v>
+      </c>
+      <c r="F22" s="14">
+        <v>651.87099999999998</v>
+      </c>
+      <c r="G22" s="14">
+        <v>559.16</v>
+      </c>
+      <c r="H22" s="43">
+        <f t="shared" si="4"/>
+        <v>598.9556</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="12">
+        <v>67.117000000000004</v>
+      </c>
+      <c r="L22" s="12">
+        <v>67.872</v>
+      </c>
+      <c r="M22" s="12">
+        <v>68.091999999999999</v>
+      </c>
+      <c r="N22" s="12">
+        <v>68.088999999999999</v>
+      </c>
+      <c r="O22" s="12">
+        <v>67.100999999999999</v>
+      </c>
+      <c r="P22" s="13">
+        <f t="shared" si="5"/>
+        <v>67.654200000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="14">
+        <v>526.38599999999997</v>
+      </c>
+      <c r="L23" s="14">
+        <v>531.13099999999997</v>
+      </c>
+      <c r="M23" s="14">
+        <v>535.15899999999999</v>
+      </c>
+      <c r="N23" s="14">
+        <v>530.67499999999995</v>
+      </c>
+      <c r="O23" s="14">
+        <v>529.73</v>
+      </c>
+      <c r="P23" s="43">
+        <f t="shared" si="5"/>
+        <v>530.61619999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="45">
+        <v>1000</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
+      <c r="J25" s="39">
+        <v>1000</v>
+      </c>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="41"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="22">
+        <v>34.709000000000003</v>
+      </c>
+      <c r="D26" s="12">
+        <v>38.118000000000002</v>
+      </c>
+      <c r="E26" s="22">
+        <v>34.709000000000003</v>
+      </c>
+      <c r="F26" s="12">
+        <v>36.225000000000001</v>
+      </c>
+      <c r="G26" s="12">
+        <v>38.567999999999998</v>
+      </c>
+      <c r="H26" s="13">
+        <f>AVERAGE(C26:G26)</f>
+        <v>36.465800000000002</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="22">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="M26" s="12">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="N26" s="22">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="O26" s="22">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="P26" s="13">
+        <f>AVERAGE(K26:O26)</f>
+        <v>0.35060000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="22">
+        <v>1447.758</v>
+      </c>
+      <c r="D27" s="12">
+        <v>1453.61</v>
+      </c>
+      <c r="E27" s="22">
+        <v>1447.758</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1435.3219999999999</v>
+      </c>
+      <c r="G27" s="12">
+        <v>1438.5519999999999</v>
+      </c>
+      <c r="H27" s="13">
+        <f t="shared" ref="H27:H29" si="6">AVERAGE(C27:G27)</f>
+        <v>1444.6</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="22">
+        <v>34.347999999999999</v>
+      </c>
+      <c r="L27" s="12">
+        <v>37.508000000000003</v>
+      </c>
+      <c r="M27" s="12">
+        <v>35.253999999999998</v>
+      </c>
+      <c r="N27" s="22">
+        <v>37.185000000000002</v>
+      </c>
+      <c r="O27" s="22">
+        <v>34.584000000000003</v>
+      </c>
+      <c r="P27" s="13">
+        <f t="shared" ref="P27:P30" si="7">AVERAGE(K27:O27)</f>
+        <v>35.775799999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="22">
+        <v>789.12300000000005</v>
+      </c>
+      <c r="D28" s="12">
+        <v>790.81</v>
+      </c>
+      <c r="E28" s="22">
+        <v>789.12300000000005</v>
+      </c>
+      <c r="F28" s="12">
+        <v>780.77499999999998</v>
+      </c>
+      <c r="G28" s="12">
+        <v>778.67399999999998</v>
+      </c>
+      <c r="H28" s="13">
+        <f t="shared" si="6"/>
+        <v>785.70100000000002</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="22">
+        <v>1215.6990000000001</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1230.0840000000001</v>
+      </c>
+      <c r="M28" s="12">
+        <v>1230.316</v>
+      </c>
+      <c r="N28" s="22">
+        <v>1210.23</v>
+      </c>
+      <c r="O28" s="22">
+        <v>1218.797</v>
+      </c>
+      <c r="P28" s="13">
+        <f t="shared" si="7"/>
+        <v>1221.0252</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="23">
+        <v>5915.4319999999998</v>
+      </c>
+      <c r="D29" s="14">
+        <v>6030.924</v>
+      </c>
+      <c r="E29" s="23">
+        <v>5915.4319999999998</v>
+      </c>
+      <c r="F29" s="14">
+        <v>6659.2470000000003</v>
+      </c>
+      <c r="G29" s="14">
+        <v>5833.2560000000003</v>
+      </c>
+      <c r="H29" s="43">
+        <f t="shared" si="6"/>
+        <v>6070.8582000000006</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" s="22">
+        <v>559.71600000000001</v>
+      </c>
+      <c r="L29" s="12">
+        <v>564.48299999999995</v>
+      </c>
+      <c r="M29" s="12">
+        <v>570.76099999999997</v>
+      </c>
+      <c r="N29" s="22">
+        <v>560.72299999999996</v>
+      </c>
+      <c r="O29" s="22">
+        <v>569.30999999999995</v>
+      </c>
+      <c r="P29" s="13">
+        <f t="shared" si="7"/>
+        <v>564.99860000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K30" s="23">
+        <v>5100.2120000000004</v>
+      </c>
+      <c r="L30" s="14">
+        <v>5033.5389999999998</v>
+      </c>
+      <c r="M30" s="14">
+        <v>5000.4139999999998</v>
+      </c>
+      <c r="N30" s="23">
+        <v>4988.5200000000004</v>
+      </c>
+      <c r="O30" s="23">
+        <v>5132.4080000000004</v>
+      </c>
+      <c r="P30" s="43">
+        <f t="shared" si="7"/>
+        <v>5051.0186000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="J18:P18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>